<commit_message>
Ajout cas de test Mouvement.ino
</commit_message>
<xml_diff>
--- a/Cas d'usage.xlsx
+++ b/Cas d'usage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offth\Documents\Etudes\Ynov\M2\IoT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cour\IOT\IOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159E16A4-2A9C-4D8F-903E-08391EF4A02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C0B10C-68E8-42BD-980C-6B97E2EDD64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{20AF6C2E-1668-46F7-A38E-9898FC19693E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20AF6C2E-1668-46F7-A38E-9898FC19693E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,65 +311,65 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,153 +713,153 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="4" width="25.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" style="1" customWidth="1"/>
     <col min="6" max="9" width="15.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="1.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="28" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="20" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="23"/>
+    <col min="13" max="13" width="11.42578125" style="15"/>
     <col min="14" max="14" width="11.42578125" style="1"/>
     <col min="15" max="27" width="25.7109375" style="1" customWidth="1"/>
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="10"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="10"/>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="22" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="35.1" customHeight="1">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="str">
+      <c r="B2" s="23" t="str">
         <f>CONCATENATE(M6," (#",N6,")")</f>
         <v>👈 Bouton gauche (#16)</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14" t="str">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23" t="str">
         <f>CONCATENATE(M9," (#",N9,")")</f>
         <v>🔊 Buzzer (#25)</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="50.1" customHeight="1">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="str">
+      <c r="B3" s="23" t="str">
         <f>CONCATENATE(M11," (#",N11,")")</f>
         <v>👉 Bouton droite  (#27)</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="14" t="str">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23" t="str">
         <f>CONCATENATE(M2," (#",N2,")")</f>
         <v>🪟 Fenêtre (#2)</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="2">
         <v>1</v>
       </c>
-      <c r="L3" s="15"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="50.1" customHeight="1">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="str">
+      <c r="B4" s="23" t="str">
         <f>CONCATENATE(M5," (#",N5,")")</f>
         <v>🏃 Détecteur de mouvement (#14)</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="str">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23" t="str">
         <f>CONCATENATE(M4," (#",N4,")")</f>
         <v>💡 LED (#12)</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="22"/>
       <c r="M4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="50.1" customHeight="1">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="str">
+      <c r="B5" s="23" t="str">
         <f>CONCATENATE(M8," (#",N8,")")</f>
         <v>💨 Détecteur de gaz (#23)</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="6" t="str">
         <f>CONCATENATE(M2," (#",N2,")")</f>
         <v>🪟 Fenêtre (#2)</v>
@@ -872,23 +872,23 @@
         <f>CONCATENATE(M9," (#",N9,")")</f>
         <v>🔊 Buzzer (#25)</v>
       </c>
-      <c r="I5" s="29" t="str">
+      <c r="I5" s="21" t="str">
         <f>CONCATENATE(M10," Rouge (#",N10,")")</f>
         <v>🔴 LED RGB Rouge (#26)</v>
       </c>
-      <c r="J5" s="15"/>
+      <c r="J5" s="22"/>
       <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="22"/>
       <c r="M5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="16">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="50.1" customHeight="1">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -903,208 +903,208 @@
         <f>CONCATENATE(M5," (#",N5,")")</f>
         <v>🏃 Détecteur de mouvement (#14)</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="18" t="str">
+      <c r="E6" s="22"/>
+      <c r="F6" s="24" t="str">
         <f>CONCATENATE(M9," (#",N9,")")</f>
         <v>🔊 Buzzer (#25)</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="30" t="str">
+      <c r="G6" s="24"/>
+      <c r="H6" s="25" t="str">
         <f>CONCATENATE(M10," Rouge (#",N10,")")</f>
         <v>🔴 LED RGB Rouge (#26)</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="22"/>
       <c r="M6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="50.1" customHeight="1">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="18" t="str">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="24" t="str">
         <f>CONCATENATE(M3," (#",N3,")")</f>
         <v>🚪 Porte (#4)</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="31" t="str">
+      <c r="G7" s="24"/>
+      <c r="H7" s="32" t="str">
         <f>CONCATENATE(M10," Vert (#",N10,")")</f>
         <v>🔴 LED RGB Vert (#26)</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="15"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="22"/>
       <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="22"/>
       <c r="M7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="16">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="50.1" customHeight="1">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14" t="str">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23" t="str">
         <f>CONCATENATE(M10," Rouge (#",N10,")")</f>
         <v>🔴 LED RGB Rouge (#26)</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="15"/>
+      <c r="L8" s="22"/>
       <c r="M8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="16">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="50.1" customHeight="1">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="str">
+      <c r="B9" s="23" t="str">
         <f>CONCATENATE(M12," (#",N12,")")</f>
         <v>🔥 Détecteur de fumée (#34)</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14" t="str">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23" t="str">
         <f>CONCATENATE(M13," (#",N13,")")</f>
         <v>🔄 Ventilo (#18)</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="2">
         <v>0</v>
       </c>
-      <c r="L9" s="15"/>
+      <c r="L9" s="22"/>
       <c r="M9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="50.1" customHeight="1">
       <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="str">
+      <c r="B10" s="29" t="str">
         <f>CONCATENATE(M7," (#",N7,")")</f>
         <v>💧 Capteur d'humidité (#17)</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14" t="str">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23" t="str">
         <f>CONCATENATE(M2," (#",N2,")")</f>
         <v>🪟 Fenêtre (#2)</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="22"/>
       <c r="M10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="16">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="50.1" customHeight="1">
       <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="32" t="str">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="30" t="str">
         <f>CONCATENATE(M10," Jaune (#",N10,")")</f>
         <v>🔴 LED RGB Jaune (#26)</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="15"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="15"/>
+      <c r="L11" s="22"/>
       <c r="M11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="16">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="50.1" customHeight="1">
       <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="14" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="27">
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="19">
         <v>0</v>
       </c>
-      <c r="L12" s="15"/>
+      <c r="L12" s="22"/>
       <c r="M12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="16">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="50.1" customHeight="1">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1114,16 +1114,16 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="27"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="3"/>
       <c r="M13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="16">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="50.1" customHeight="1">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1133,10 +1133,10 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="27"/>
+      <c r="K14" s="19"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="50.1" customHeight="1">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1146,10 +1146,10 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="27"/>
+      <c r="K15" s="19"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="50.1" customHeight="1">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1159,10 +1159,10 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="27"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="50.1" customHeight="1">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1172,10 +1172,10 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="27"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="50.1" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1185,10 +1185,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="27"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="50.1" customHeight="1">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
@@ -1198,25 +1198,17 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="27"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="L2:L12"/>
-    <mergeCell ref="J2:J12"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:I12"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="F9:I9"/>
@@ -1228,6 +1220,14 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B8:D8"/>
+    <mergeCell ref="L2:L12"/>
+    <mergeCell ref="J2:J12"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:I12"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>

</xml_diff>

<commit_message>
Ajout GAZ / VAPEUR / LED
</commit_message>
<xml_diff>
--- a/Cas d'usage.xlsx
+++ b/Cas d'usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cour\IOT\IOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C7F53-5804-4B13-8148-4EFDC9B258CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66230BFA-01D3-46B1-A797-98E30F9CC55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20AF6C2E-1668-46F7-A38E-9898FC19693E}"/>
   </bookViews>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED2B8E5-605C-42CE-8DCF-A8A120E0360C}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="105" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -764,8 +764,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="str">
-        <f>CONCATENATE(M6," (#",N6,")")</f>
-        <v>👈 Bouton gauche (#16)</v>
+        <f>CONCATENATE(M11," (#",N11,")")</f>
+        <v>👉 Bouton droite  (#27)</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -794,8 +794,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="str">
-        <f>CONCATENATE(M11," (#",N11,")")</f>
-        <v>👉 Bouton droite  (#27)</v>
+        <f>CONCATENATE(M6," (#",N6,")")</f>
+        <v>👈 Bouton gauche (#16)</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>

</xml_diff>